<commit_message>
made Point use smart-pointer-to-impl
</commit_message>
<xml_diff>
--- a/cpp/times.xlsx
+++ b/cpp/times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\.spyder-py3\Robert_Python\Walk_Finder\cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2094DF7E-3A9D-46C9-904F-525D1D63212E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5DD2B-ADE4-4B1C-9BF0-91F114241075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>No opimizations:</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Small Triangle</t>
+  </si>
+  <si>
+    <t>Points On Line</t>
+  </si>
+  <si>
+    <t>Smart Pointer to Implementation</t>
   </si>
 </sst>
 </file>
@@ -83,10 +89,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,19 +384,33 @@
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -406,61 +426,159 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>313</v>
       </c>
       <c r="C3">
         <v>1067</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>173</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>327</v>
       </c>
       <c r="C4">
         <v>1067</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>163</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>317</v>
       </c>
       <c r="C5">
         <v>1059</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>163</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>285</v>
       </c>
       <c r="C6">
         <v>1112</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>155</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>278</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1220</v>
+      </c>
+      <c r="D7">
+        <v>172</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f>AVERAGE(B3:B7)</f>
         <v>304</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f>AVERAGE(C3:C7)</f>
-        <v>1076.25</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>1105</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:L9" si="0">AVERAGE(D3:D7)</f>
+        <v>165.2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>23.6</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>1016.6</v>
+      </c>
+      <c r="H9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tried out ways to reduce number of cells needed for PointStore
</commit_message>
<xml_diff>
--- a/cpp/times.xlsx
+++ b/cpp/times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\.spyder-py3\Robert_Python\Walk_Finder\cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5DD2B-ADE4-4B1C-9BF0-91F114241075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B1B17D-B1CF-48E1-98DE-9DAF9B8FAA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,6 +461,9 @@
       <c r="F3">
         <v>1004</v>
       </c>
+      <c r="L3">
+        <v>1046</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -570,9 +573,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>1046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>